<commit_message>
End of Writing Sprint
1500 odd words written.
Family is home so time to pull the pin.
</commit_message>
<xml_diff>
--- a/Tables/Tables.xlsx
+++ b/Tables/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17760" yWindow="460" windowWidth="33440" windowHeight="31540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="32000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Response Times" sheetId="5" r:id="rId1"/>
@@ -313,9 +313,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="178">
+  <cellStyleXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,7 +510,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="178">
+  <cellStyles count="180">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -597,6 +599,7 @@
     <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -685,6 +688,7 @@
     <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -963,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" zoomScalePageLayoutView="186" workbookViewId="0">
+    <sheetView zoomScale="186" zoomScaleNormal="186" zoomScalePageLayoutView="186" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1127,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="186" zoomScaleNormal="186" zoomScalePageLayoutView="186" workbookViewId="0">
-      <selection sqref="A1:B56"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="186" zoomScaleNormal="186" zoomScalePageLayoutView="186" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,175 +1150,175 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4">
-        <v>0.90625</v>
+        <v>0.987915407854984</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.98198198198198194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4">
-        <v>0.98809523809523792</v>
+        <v>1.0106382978723401</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4">
-        <v>0.98355263157894701</v>
+        <v>1.0103092783505101</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.99004975124378103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.98759305210918102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4">
-        <v>0.96977329974811</v>
+        <v>0.97643097643097609</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
-        <v>0.90625</v>
+        <v>0.98989898989898906</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.97305389221556793</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B11" s="4">
-        <v>0.86363636363636298</v>
+        <v>0.98214285714285698</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
-        <v>0.97643097643097609</v>
+        <v>0.96977329974811</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.97887323943661897</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4">
-        <v>0.97887323943661897</v>
+        <v>0.99451553930530101</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4">
-        <v>2.8846153846153803E-2</v>
+        <v>0.99323181049069309</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.95652173913043403</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4">
-        <v>0.98759305210918102</v>
+        <v>0.96969696969696895</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.95652173913043403</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4">
-        <v>0.98989898989898906</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.90625</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4">
-        <v>0.98850574712643602</v>
+        <v>0.90909090909090906</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B22" s="4">
-        <v>0.98847926267281094</v>
+        <v>0.86363636363636298</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5">
         <v>0</v>
@@ -1322,111 +1326,111 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="4">
-        <v>0.99456521739130399</v>
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B25" s="4">
-        <v>0.99763033175355398</v>
+        <v>0.83870967741935398</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="4">
-        <v>0.9375</v>
+        <v>4</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4">
-        <v>0.98198198198198194</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B28" s="4">
-        <v>0.99453551912568305</v>
+        <v>0.96551724137931005</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.90625</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="4">
-        <v>0.99004975124378103</v>
+        <v>43</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B31" s="4">
-        <v>1.0103092783505101</v>
+        <v>0.98850574712643602</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B32" s="4">
-        <v>0.99723756906077299</v>
+        <v>0.98355263157894701</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4">
-        <v>0.987915407854984</v>
+        <v>8.3333333333333297E-3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="5">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.99723756906077299</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B35" s="4">
-        <v>0.99300699300699302</v>
+        <v>0.98630136986301298</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B36" s="4">
-        <v>0.90909090909090906</v>
+        <v>0.99453551912568305</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B37" s="5">
         <v>1</v>
@@ -1434,157 +1438,160 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="4">
-        <v>0.96551724137931005</v>
+        <v>7</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="4">
-        <v>0.9882629107981219</v>
+        <v>8</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="4">
-        <v>0.99323181049069309</v>
+        <v>19</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B41" s="4">
-        <v>0.97305389221556793</v>
+        <v>0.99300699300699302</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="5">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.98847926267281094</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1.0106382978723401</v>
+        <v>14</v>
+      </c>
+      <c r="B43" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B44" s="4">
-        <v>0.99456521739130399</v>
+        <v>0.99543378995433696</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B45" s="4">
-        <v>0.96969696969696895</v>
+        <v>2.8846153846153803E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B46" s="4">
-        <v>0.99451553930530101</v>
+        <v>1.26182965299684E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B47" s="4">
-        <v>0.83870967741935398</v>
+        <v>0.99727520435967199</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4">
-        <v>0.9375</v>
+        <v>0.99456521739130399</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B49" s="4">
-        <v>8.3333333333333297E-3</v>
+        <v>0.99456521739130399</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="4">
-        <v>1.26182965299684E-2</v>
+        <v>38</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B51" s="4">
-        <v>3.6269430051813399E-2</v>
+        <v>0.98809523809523792</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="4">
-        <v>0.99727520435967199</v>
+        <v>21</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B53" s="4">
-        <v>0.98214285714285698</v>
+        <v>0.99763033175355398</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B54" s="4">
-        <v>3.4768211920529798E-2</v>
+        <v>0.9882629107981219</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B55" s="4">
-        <v>0.98630136986301298</v>
+        <v>3.6269430051813399E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4">
-        <v>0.99543378995433696</v>
+        <v>3.4768211920529798E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B56">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>